<commit_message>
Atualizado IG x IE
</commit_message>
<xml_diff>
--- a/outputs/sisaprophelper#autoaprop/autoapropxlsx/IG.XLSX
+++ b/outputs/sisaprophelper#autoaprop/autoapropxlsx/IG.XLSX
@@ -136,9 +136,6 @@
     <t>2657</t>
   </si>
   <si>
-    <t>2664</t>
-  </si>
-  <si>
     <t>2851</t>
   </si>
   <si>
@@ -211,6 +208,9 @@
     <t> </t>
   </si>
   <si>
+    <t> </t>
+  </si>
+  <si>
     <t>PAULO SERGIO POGGIAN</t>
   </si>
   <si>
@@ -220,9 +220,6 @@
     <t>ANA MARIA DA COSTA FERREIRA</t>
   </si>
   <si>
-    <t>HELENICE DE JESUS PEREIRA</t>
-  </si>
-  <si>
     <t>TOMAZ GONCALVES DA F FILHO</t>
   </si>
   <si>
@@ -254,6 +251,9 @@
   </si>
   <si>
     <t>JOYCE DE FIGUEIREDO FERREIRA</t>
+  </si>
+  <si>
+    <t> </t>
   </si>
   <si>
     <t> </t>

</xml_diff>